<commit_message>
add grouped variance datasets + signatures
</commit_message>
<xml_diff>
--- a/data/original_data/data_dictionary_anomaly_v20240105.xlsx
+++ b/data/original_data/data_dictionary_anomaly_v20240105.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anjaadamov/Documents/projects/12_infant_gut/meta-infant-gut-dvpmt/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamova/Documents/projects/14_LM1/NJODE/Probabilistic_forecasting_for_Anomaly_Detection/data/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D85060-8539-B54D-B044-581505FA5E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96375327-A3B1-2842-BDFE-EEFFA4B832D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1500" windowWidth="22840" windowHeight="18560" activeTab="1" xr2:uid="{0751DAF1-5C18-FB4D-876E-E89AC4BC8475}"/>
+    <workbookView xWindow="13460" yWindow="1300" windowWidth="22840" windowHeight="18560" activeTab="3" xr2:uid="{0751DAF1-5C18-FB4D-876E-E89AC4BC8475}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -499,62 +499,62 @@
     <t>otu__*</t>
   </si>
   <si>
-    <t>Relative abundance of microbial OTUs where low abundance OTUs were grouped: if OTU relative abundance &lt;1e-3 for &gt;= 0.9 samples it was grouped to "otu__other_rare".</t>
+    <t>sampling_depth</t>
+  </si>
+  <si>
+    <t>Measure of microbial feature uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The smaller the sampling depth the noisier we assume the obtained microbial relative abundances are. </t>
+  </si>
+  <si>
+    <t>[1009, 510789]</t>
+  </si>
+  <si>
+    <t>age_months_rounded05</t>
+  </si>
+  <si>
+    <t>age_months_rounded1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age of infant at time of sampling rounded in full months. </t>
+  </si>
+  <si>
+    <t>div_alpha_shannon</t>
+  </si>
+  <si>
+    <t>div_alpha_observed_features</t>
+  </si>
+  <si>
+    <t>div_alpha_faith_pd</t>
+  </si>
+  <si>
+    <t>[0.0, 6.038928]</t>
+  </si>
+  <si>
+    <t>Microbial summary feature</t>
+  </si>
+  <si>
+    <t>Faith’s phylogenetic diversity describing within sample diversity by  incorporating phylogenetic difference between species.</t>
+  </si>
+  <si>
+    <t>Shannon diversity index describing within sample diversity while accounting for both abundance anv evenness of the taxa present.</t>
+  </si>
+  <si>
+    <t>Quantification of within sample diversity by number of distinct features observed.</t>
+  </si>
+  <si>
+    <t>[1.0, 133.05]</t>
+  </si>
+  <si>
+    <t>[1.837224, 43.060240]</t>
   </si>
   <si>
     <t>Relative abundance of microbial features grouped on taxonomic genus (or if unknown family) level with SILVA reference database.
-Genus with relative abundance &lt;1e-4 for &gt;= 0.9 samples was grouped to "g__other_rare".</t>
-  </si>
-  <si>
-    <t>sampling_depth</t>
-  </si>
-  <si>
-    <t>Measure of microbial feature uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The smaller the sampling depth the noisier we assume the obtained microbial relative abundances are. </t>
-  </si>
-  <si>
-    <t>[1009, 510789]</t>
-  </si>
-  <si>
-    <t>age_months_rounded05</t>
-  </si>
-  <si>
-    <t>age_months_rounded1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age of infant at time of sampling rounded in full months. </t>
-  </si>
-  <si>
-    <t>div_alpha_shannon</t>
-  </si>
-  <si>
-    <t>div_alpha_observed_features</t>
-  </si>
-  <si>
-    <t>div_alpha_faith_pd</t>
-  </si>
-  <si>
-    <t>[0.0, 6.038928]</t>
-  </si>
-  <si>
-    <t>Microbial summary feature</t>
-  </si>
-  <si>
-    <t>Faith’s phylogenetic diversity describing within sample diversity by  incorporating phylogenetic difference between species.</t>
-  </si>
-  <si>
-    <t>Shannon diversity index describing within sample diversity while accounting for both abundance anv evenness of the taxa present.</t>
-  </si>
-  <si>
-    <t>Quantification of within sample diversity by number of distinct features observed.</t>
-  </si>
-  <si>
-    <t>[1.0, 133.05]</t>
-  </si>
-  <si>
-    <t>[1.837224, 43.060240]</t>
+Genus with relative abundance &lt;1e-4 for &gt;= 0.9 samples was grouped to "g__other_rare". Low variance features were grouped into "g__low_var".</t>
+  </si>
+  <si>
+    <t>Relative abundance of microbial OTUs where low abundance OTUs were grouped: if OTU relative abundance &lt;1e-3 for &gt;= 0.9 samples it was grouped to "otu__other_rare". Low variance features were grouped into "otu__low_var".</t>
   </si>
 </sst>
 </file>
@@ -684,9 +684,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -724,7 +724,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -830,7 +830,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -972,7 +972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1319,9 +1319,9 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>52</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>52</v>
@@ -1546,7 +1546,7 @@
         <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>57</v>
@@ -1812,7 +1812,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>100</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>95</v>
@@ -1834,27 +1834,27 @@
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
@@ -1863,18 +1863,18 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1883,33 +1883,33 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1927,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD29"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>52</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>52</v>
@@ -2152,7 +2152,7 @@
         <v>53</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>57</v>
@@ -2418,7 +2418,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>101</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>95</v>
@@ -2440,27 +2440,27 @@
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
@@ -2469,18 +2469,18 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -2489,33 +2489,33 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2531,7 +2531,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ADD: grouped variance datasets + signatures (`V20240105`) (#2)
* add grouped variance datasets + signatures

* include all fts in signature if they meet restrictions

* add lowvarq94 as low-dim option
</commit_message>
<xml_diff>
--- a/data/original_data/data_dictionary_anomaly_v20240105.xlsx
+++ b/data/original_data/data_dictionary_anomaly_v20240105.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anjaadamov/Documents/projects/12_infant_gut/meta-infant-gut-dvpmt/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamova/Documents/projects/14_LM1/NJODE/Probabilistic_forecasting_for_Anomaly_Detection/data/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D85060-8539-B54D-B044-581505FA5E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96375327-A3B1-2842-BDFE-EEFFA4B832D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1500" windowWidth="22840" windowHeight="18560" activeTab="1" xr2:uid="{0751DAF1-5C18-FB4D-876E-E89AC4BC8475}"/>
+    <workbookView xWindow="13460" yWindow="1300" windowWidth="22840" windowHeight="18560" activeTab="3" xr2:uid="{0751DAF1-5C18-FB4D-876E-E89AC4BC8475}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -499,62 +499,62 @@
     <t>otu__*</t>
   </si>
   <si>
-    <t>Relative abundance of microbial OTUs where low abundance OTUs were grouped: if OTU relative abundance &lt;1e-3 for &gt;= 0.9 samples it was grouped to "otu__other_rare".</t>
+    <t>sampling_depth</t>
+  </si>
+  <si>
+    <t>Measure of microbial feature uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The smaller the sampling depth the noisier we assume the obtained microbial relative abundances are. </t>
+  </si>
+  <si>
+    <t>[1009, 510789]</t>
+  </si>
+  <si>
+    <t>age_months_rounded05</t>
+  </si>
+  <si>
+    <t>age_months_rounded1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age of infant at time of sampling rounded in full months. </t>
+  </si>
+  <si>
+    <t>div_alpha_shannon</t>
+  </si>
+  <si>
+    <t>div_alpha_observed_features</t>
+  </si>
+  <si>
+    <t>div_alpha_faith_pd</t>
+  </si>
+  <si>
+    <t>[0.0, 6.038928]</t>
+  </si>
+  <si>
+    <t>Microbial summary feature</t>
+  </si>
+  <si>
+    <t>Faith’s phylogenetic diversity describing within sample diversity by  incorporating phylogenetic difference between species.</t>
+  </si>
+  <si>
+    <t>Shannon diversity index describing within sample diversity while accounting for both abundance anv evenness of the taxa present.</t>
+  </si>
+  <si>
+    <t>Quantification of within sample diversity by number of distinct features observed.</t>
+  </si>
+  <si>
+    <t>[1.0, 133.05]</t>
+  </si>
+  <si>
+    <t>[1.837224, 43.060240]</t>
   </si>
   <si>
     <t>Relative abundance of microbial features grouped on taxonomic genus (or if unknown family) level with SILVA reference database.
-Genus with relative abundance &lt;1e-4 for &gt;= 0.9 samples was grouped to "g__other_rare".</t>
-  </si>
-  <si>
-    <t>sampling_depth</t>
-  </si>
-  <si>
-    <t>Measure of microbial feature uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The smaller the sampling depth the noisier we assume the obtained microbial relative abundances are. </t>
-  </si>
-  <si>
-    <t>[1009, 510789]</t>
-  </si>
-  <si>
-    <t>age_months_rounded05</t>
-  </si>
-  <si>
-    <t>age_months_rounded1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age of infant at time of sampling rounded in full months. </t>
-  </si>
-  <si>
-    <t>div_alpha_shannon</t>
-  </si>
-  <si>
-    <t>div_alpha_observed_features</t>
-  </si>
-  <si>
-    <t>div_alpha_faith_pd</t>
-  </si>
-  <si>
-    <t>[0.0, 6.038928]</t>
-  </si>
-  <si>
-    <t>Microbial summary feature</t>
-  </si>
-  <si>
-    <t>Faith’s phylogenetic diversity describing within sample diversity by  incorporating phylogenetic difference between species.</t>
-  </si>
-  <si>
-    <t>Shannon diversity index describing within sample diversity while accounting for both abundance anv evenness of the taxa present.</t>
-  </si>
-  <si>
-    <t>Quantification of within sample diversity by number of distinct features observed.</t>
-  </si>
-  <si>
-    <t>[1.0, 133.05]</t>
-  </si>
-  <si>
-    <t>[1.837224, 43.060240]</t>
+Genus with relative abundance &lt;1e-4 for &gt;= 0.9 samples was grouped to "g__other_rare". Low variance features were grouped into "g__low_var".</t>
+  </si>
+  <si>
+    <t>Relative abundance of microbial OTUs where low abundance OTUs were grouped: if OTU relative abundance &lt;1e-3 for &gt;= 0.9 samples it was grouped to "otu__other_rare". Low variance features were grouped into "otu__low_var".</t>
   </si>
 </sst>
 </file>
@@ -684,9 +684,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -724,7 +724,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -830,7 +830,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -972,7 +972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1319,9 +1319,9 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>52</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>52</v>
@@ -1546,7 +1546,7 @@
         <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>57</v>
@@ -1812,7 +1812,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>100</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>95</v>
@@ -1834,27 +1834,27 @@
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
@@ -1863,18 +1863,18 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1883,33 +1883,33 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1927,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD29"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>52</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>52</v>
@@ -2152,7 +2152,7 @@
         <v>53</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>57</v>
@@ -2418,7 +2418,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>101</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>95</v>
@@ -2440,27 +2440,27 @@
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
@@ -2469,18 +2469,18 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -2489,33 +2489,33 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2531,7 +2531,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>